<commit_message>
add Embrace to the sheet
Example of timing perturbation canceling the effect
</commit_message>
<xml_diff>
--- a/Ele Haste Value Visualization - P2 Variations.xlsx
+++ b/Ele Haste Value Visualization - P2 Variations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paul\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{93634669-B858-4BE3-B4FC-315BE0DA6995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D04F7AE-22E0-4564-948A-0FE8D0EB902C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="-110" windowWidth="37220" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,12 +19,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">DPSChart!$A$1:$C$8001</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Phase</t>
   </si>
@@ -42,6 +55,12 @@
   </si>
   <si>
     <t>DPS - 1ms delay No Overwrite</t>
+  </si>
+  <si>
+    <t>Embrace of the Spider - 300ms delay No Overwrite</t>
+  </si>
+  <si>
+    <t>Embrace, +250dps Normalized</t>
   </si>
 </sst>
 </file>
@@ -642,6 +661,15 @@
               <a:rPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
               <a:t>Max wait for LvB/FS (ms)" and "Allow Flameshock to be overwritten"</a:t>
             </a:r>
+          </a:p>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1050" b="0" i="0" u="none" strike="noStrike" baseline="0"/>
+              <a:t>Phase 2 (Ulduar BiS), with bonus Haste subtracted/added</a:t>
+            </a:r>
             <a:endParaRPr lang="en-US" sz="1050"/>
           </a:p>
         </c:rich>
@@ -5650,6 +5678,640 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-31C5-463C-B0D2-5A10A47A92D4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Embrace of the Spider, Normalized</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>DPSChart!$H$2:$H$201</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="200"/>
+                <c:pt idx="0">
+                  <c:v>10355.6726806803</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10355.888014902799</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10356.340729658699</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10359.7109243265</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>10359.9107656095</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10362.4457653606</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>10364.318810303699</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>10366.744244468</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>10368.3092300516</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>10369.927840189201</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10374.7390280158</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10376.400067599599</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10378.5326106266</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10384.0178379795</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>10385.4170001859</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10389.328551262101</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>10392.4202839256</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>10394.9942426785</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>10395.076047549301</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>10397.648197570101</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>10400.3337507491</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>10402.1998094103</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>10405.2866116727</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>10406.230553864099</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>10408.567273865199</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>10409.763398694</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>10411.395012421999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>10412.871432989799</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>10415.1955221922</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>10416.3908166205</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>10418.696903980301</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>10418.3252408031</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>10417.703715719599</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10418.814466719699</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>10420.8074874168</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>10421.788182861799</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>10429.1718358906</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>10430.567604600001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>10433.2813169568</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>10434.514737798399</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>10436.105315352201</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>10437.395649853799</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10438.286013412901</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>10442.3637837687</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>10444.671775360999</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>10445.026861612399</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>10445.2861676581</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>10447.898176176401</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>10449.3004224214</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>10453.6478648471</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>10454.9537918487</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>10456.598585469401</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10462.9475250449</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>10466.2090250244</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>10468.672107022499</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>10471.0473502516</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>10472.0736175498</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>10473.4167269397</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>10474.797663306101</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>10477.181025051799</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>10479.0820640689</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>10481.137285988299</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>10481.490956043501</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>10484.624123620501</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>10485.6192069972</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>10488.9043390607</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>10489.8697324719</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>10491.4919261345</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>10493.3103938843</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>10494.3115554263</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>10495.6809079923</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>10497.722524750599</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>10498.822897428699</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>10501.8246469969</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>10502.110829823099</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>10504.996519313399</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>10506.841079858999</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>10508.4664597889</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>10510.5622390523</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>10512.4979073418</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>10513.255799903</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>10513.5369620276</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>10514.8513878386</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>10517.5707432992</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>10519.7681720949</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>10521.828701767499</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>10522.840250564799</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>10525.5392716729</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>10527.6970693888</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>10530.3730581666</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>10532.220688085699</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>10537.382520401999</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>10537.0201261163</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>10539.343660242899</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>10541.0924515684</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>10544.077044742</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>10544.9792953412</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>10545.0147771591</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>10547.528430341899</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>10554.752923951401</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>10555.969206984701</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>10556.539899203401</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>10560.171561777501</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>10560.027477101299</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>10562.5038857241</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>10564.344527584601</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>10566.096586939801</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>10566.675593088699</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>10568.1965946981</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>10568.949248574199</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>10572.575064028801</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>10573.9884536676</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>10575.1337880561</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>10575.5685118662</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>10578.3999890135</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>10584.2928116802</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>10587.298214152999</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>10588.9876178268</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>10592.542461840399</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>10594.9635867711</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>10598.767489850699</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>10600.1570545782</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>10603.480684903099</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>10605.8003239725</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>10609.603456565201</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>10609.999239895</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>10612.603643853099</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>10614.9456265115</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>10617.4443818871</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>10618.9008909686</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>10620.978256724</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>10620.606307488601</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>10623.681531623</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>10624.504665611799</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>10626.782421722201</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>10627.856266660399</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>10630.716666599499</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>10632.4224503655</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>10632.8886949358</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>10632.758545761901</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>10634.4230431625</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>10637.8157569714</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>10639.971251504399</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>10643.3374825174</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>10647.2473597341</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>10648.3713028494</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>10652.5779359758</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>10651.638711788701</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>10652.617326940401</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>10653.339929924799</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>10655.5663599255</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>10657.1692824561</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>10659.2619717746</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>10662.523529529301</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>10662.0962361152</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>10664.2135989013</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>10665.2456187099</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>10667.683503717501</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>10667.6849614695</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>10669.072136762599</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>10670.910868978401</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>10673.4412289885</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>10674.3086405269</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>10675.7055090699</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>10679.6833434032</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>10680.994719037701</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>10681.571631062199</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>10683.7683958903</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>10686.455650457799</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>10687.7873299864</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>10689.100630765401</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>10688.6638213608</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>10691.6303143202</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>10693.5487349295</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>10694.6362803506</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>10694.104440569699</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>10696.295503564699</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>10697.824409697099</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>10698.645411998101</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>10698.680845298</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>10700.373830722099</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>10702.8365372587</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>10719.207615003899</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>10720.083836741</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>10722.3239580684</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>10725.802054919101</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>10729.3646399017</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>10733.0556590214</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>10735.286108345301</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>10736.0186487343</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>10737.626864178899</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>10740.9001293487</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>10741.4825528355</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>10742.285455421699</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>10748.6540684875</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>10751.3522980869</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>10752.242887620199</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>10754.678460952</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>10756.483021178499</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>10759.171333975901</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{000000C8-31C5-463C-B0D2-5A10A47A92D4}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -6751,10 +7413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F201"/>
+  <dimension ref="A1:H201"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6764,9 +7426,10 @@
     <col min="4" max="4" width="13.90625" customWidth="1"/>
     <col min="5" max="5" width="11.453125" customWidth="1"/>
     <col min="6" max="6" width="11" customWidth="1"/>
+    <col min="7" max="7" width="15.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6785,8 +7448,14 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>2</v>
       </c>
@@ -6805,8 +7474,15 @@
       <c r="F2">
         <v>10342.4855307547</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G2">
+        <v>10105.6726806803</v>
+      </c>
+      <c r="H2">
+        <f>G2+250</f>
+        <v>10355.6726806803</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6825,8 +7501,15 @@
       <c r="F3">
         <v>10345.9013795353</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3">
+        <v>10105.888014902799</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H66" si="0">G3+250</f>
+        <v>10355.888014902799</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -6845,8 +7528,15 @@
       <c r="F4">
         <v>10344.7557932905</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G4">
+        <v>10106.340729658699</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>10356.340729658699</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>2</v>
       </c>
@@ -6865,8 +7555,15 @@
       <c r="F5">
         <v>10344.330850959401</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G5">
+        <v>10109.7109243265</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>10359.7109243265</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>2</v>
       </c>
@@ -6885,8 +7582,15 @@
       <c r="F6">
         <v>10346.6078117832</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G6">
+        <v>10109.9107656095</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>10359.9107656095</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>2</v>
       </c>
@@ -6905,8 +7609,15 @@
       <c r="F7">
         <v>10345.9222368592</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G7">
+        <v>10112.4457653606</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>10362.4457653606</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>2</v>
       </c>
@@ -6925,8 +7636,15 @@
       <c r="F8">
         <v>10345.430556367901</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G8">
+        <v>10114.318810303699</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>10364.318810303699</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -6945,8 +7663,15 @@
       <c r="F9">
         <v>10345.704829434</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G9">
+        <v>10116.744244468</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>10366.744244468</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>2</v>
       </c>
@@ -6965,8 +7690,15 @@
       <c r="F10">
         <v>10346.7142350302</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10">
+        <v>10118.3092300516</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>10368.3092300516</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>2</v>
       </c>
@@ -6985,8 +7717,15 @@
       <c r="F11">
         <v>10348.4567918927</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G11">
+        <v>10119.927840189201</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>10369.927840189201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -7005,8 +7744,15 @@
       <c r="F12">
         <v>10349.1289863822</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G12">
+        <v>10124.7390280158</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>10374.7390280158</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -7025,8 +7771,15 @@
       <c r="F13">
         <v>10348.4195897802</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G13">
+        <v>10126.400067599599</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>10376.400067599599</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>2</v>
       </c>
@@ -7045,8 +7798,15 @@
       <c r="F14">
         <v>10355.643163664299</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G14">
+        <v>10128.5326106266</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>10378.5326106266</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -7065,8 +7825,15 @@
       <c r="F15">
         <v>10355.193778459299</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G15">
+        <v>10134.0178379795</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>10384.0178379795</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -7085,8 +7852,15 @@
       <c r="F16">
         <v>10357.794991527</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G16">
+        <v>10135.4170001859</v>
+      </c>
+      <c r="H16">
+        <f t="shared" si="0"/>
+        <v>10385.4170001859</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -7105,8 +7879,15 @@
       <c r="F17">
         <v>10373.803698203201</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G17">
+        <v>10139.328551262101</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="0"/>
+        <v>10389.328551262101</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>2</v>
       </c>
@@ -7125,8 +7906,15 @@
       <c r="F18">
         <v>10408.401617252501</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G18">
+        <v>10142.4202839256</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="0"/>
+        <v>10392.4202839256</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>2</v>
       </c>
@@ -7145,8 +7933,15 @@
       <c r="F19">
         <v>10408.2710613368</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G19">
+        <v>10144.9942426785</v>
+      </c>
+      <c r="H19">
+        <f t="shared" si="0"/>
+        <v>10394.9942426785</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>2</v>
       </c>
@@ -7165,8 +7960,15 @@
       <c r="F20">
         <v>10407.9309494141</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G20">
+        <v>10145.076047549301</v>
+      </c>
+      <c r="H20">
+        <f t="shared" si="0"/>
+        <v>10395.076047549301</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>2</v>
       </c>
@@ -7185,8 +7987,15 @@
       <c r="F21">
         <v>10414.231529862</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G21">
+        <v>10147.648197570101</v>
+      </c>
+      <c r="H21">
+        <f t="shared" si="0"/>
+        <v>10397.648197570101</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>2</v>
       </c>
@@ -7205,8 +8014,15 @@
       <c r="F22">
         <v>10413.078988949799</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22">
+        <v>10150.3337507491</v>
+      </c>
+      <c r="H22">
+        <f t="shared" si="0"/>
+        <v>10400.3337507491</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>2</v>
       </c>
@@ -7225,8 +8041,15 @@
       <c r="F23">
         <v>10414.864762884999</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G23">
+        <v>10152.1998094103</v>
+      </c>
+      <c r="H23">
+        <f t="shared" si="0"/>
+        <v>10402.1998094103</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -7245,8 +8068,15 @@
       <c r="F24">
         <v>10412.431110691599</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G24">
+        <v>10155.2866116727</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="0"/>
+        <v>10405.2866116727</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>2</v>
       </c>
@@ -7265,8 +8095,15 @@
       <c r="F25">
         <v>10413.199342927601</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25">
+        <v>10156.230553864099</v>
+      </c>
+      <c r="H25">
+        <f t="shared" si="0"/>
+        <v>10406.230553864099</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -7285,8 +8122,15 @@
       <c r="F26">
         <v>10412.0719207197</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G26">
+        <v>10158.567273865199</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="0"/>
+        <v>10408.567273865199</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>2</v>
       </c>
@@ -7305,8 +8149,15 @@
       <c r="F27">
         <v>10413.916191295601</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G27">
+        <v>10159.763398694</v>
+      </c>
+      <c r="H27">
+        <f t="shared" si="0"/>
+        <v>10409.763398694</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>2</v>
       </c>
@@ -7325,8 +8176,15 @@
       <c r="F28">
         <v>10414.5440959405</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G28">
+        <v>10161.395012421999</v>
+      </c>
+      <c r="H28">
+        <f t="shared" si="0"/>
+        <v>10411.395012421999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -7345,8 +8203,15 @@
       <c r="F29">
         <v>10415.464870916199</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G29">
+        <v>10162.871432989799</v>
+      </c>
+      <c r="H29">
+        <f t="shared" si="0"/>
+        <v>10412.871432989799</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -7365,8 +8230,15 @@
       <c r="F30">
         <v>10414.784202815899</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G30">
+        <v>10165.1955221922</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="0"/>
+        <v>10415.1955221922</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>2</v>
       </c>
@@ -7385,8 +8257,15 @@
       <c r="F31">
         <v>10415.434337909899</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G31">
+        <v>10166.3908166205</v>
+      </c>
+      <c r="H31">
+        <f t="shared" si="0"/>
+        <v>10416.3908166205</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>2</v>
       </c>
@@ -7405,8 +8284,15 @@
       <c r="F32">
         <v>10414.6430223159</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G32">
+        <v>10168.696903980301</v>
+      </c>
+      <c r="H32">
+        <f t="shared" si="0"/>
+        <v>10418.696903980301</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>2</v>
       </c>
@@ -7425,8 +8311,15 @@
       <c r="F33">
         <v>10417.1728339539</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G33">
+        <v>10168.3252408031</v>
+      </c>
+      <c r="H33">
+        <f t="shared" si="0"/>
+        <v>10418.3252408031</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>2</v>
       </c>
@@ -7445,8 +8338,15 @@
       <c r="F34">
         <v>10416.5197341562</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G34">
+        <v>10167.703715719599</v>
+      </c>
+      <c r="H34">
+        <f t="shared" si="0"/>
+        <v>10417.703715719599</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>2</v>
       </c>
@@ -7465,8 +8365,15 @@
       <c r="F35">
         <v>10414.6869137786</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G35">
+        <v>10168.814466719699</v>
+      </c>
+      <c r="H35">
+        <f t="shared" si="0"/>
+        <v>10418.814466719699</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>2</v>
       </c>
@@ -7485,8 +8392,15 @@
       <c r="F36">
         <v>10427.5400851591</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <v>10170.8074874168</v>
+      </c>
+      <c r="H36">
+        <f t="shared" si="0"/>
+        <v>10420.8074874168</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>2</v>
       </c>
@@ -7505,8 +8419,15 @@
       <c r="F37">
         <v>10403.4570204186</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G37">
+        <v>10171.788182861799</v>
+      </c>
+      <c r="H37">
+        <f t="shared" si="0"/>
+        <v>10421.788182861799</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>2</v>
       </c>
@@ -7525,8 +8446,15 @@
       <c r="F38">
         <v>10406.110452151101</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <v>10179.1718358906</v>
+      </c>
+      <c r="H38">
+        <f t="shared" si="0"/>
+        <v>10429.1718358906</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>2</v>
       </c>
@@ -7545,8 +8473,15 @@
       <c r="F39">
         <v>10406.8268607299</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G39">
+        <v>10180.567604600001</v>
+      </c>
+      <c r="H39">
+        <f t="shared" si="0"/>
+        <v>10430.567604600001</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>2</v>
       </c>
@@ -7565,8 +8500,15 @@
       <c r="F40">
         <v>10406.307533457501</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G40">
+        <v>10183.2813169568</v>
+      </c>
+      <c r="H40">
+        <f t="shared" si="0"/>
+        <v>10433.2813169568</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>2</v>
       </c>
@@ -7585,8 +8527,15 @@
       <c r="F41">
         <v>10405.861635704599</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G41">
+        <v>10184.514737798399</v>
+      </c>
+      <c r="H41">
+        <f t="shared" si="0"/>
+        <v>10434.514737798399</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>2</v>
       </c>
@@ -7605,8 +8554,15 @@
       <c r="F42">
         <v>10405.4759046705</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G42">
+        <v>10186.105315352201</v>
+      </c>
+      <c r="H42">
+        <f t="shared" si="0"/>
+        <v>10436.105315352201</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>2</v>
       </c>
@@ -7625,8 +8581,15 @@
       <c r="F43">
         <v>10405.440665078801</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G43">
+        <v>10187.395649853799</v>
+      </c>
+      <c r="H43">
+        <f t="shared" si="0"/>
+        <v>10437.395649853799</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>2</v>
       </c>
@@ -7645,8 +8608,15 @@
       <c r="F44">
         <v>10405.0644637352</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G44">
+        <v>10188.286013412901</v>
+      </c>
+      <c r="H44">
+        <f t="shared" si="0"/>
+        <v>10438.286013412901</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>2</v>
       </c>
@@ -7665,8 +8635,15 @@
       <c r="F45">
         <v>10404.655206535999</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G45">
+        <v>10192.3637837687</v>
+      </c>
+      <c r="H45">
+        <f t="shared" si="0"/>
+        <v>10442.3637837687</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>2</v>
       </c>
@@ -7685,8 +8662,15 @@
       <c r="F46">
         <v>10449.056488293099</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G46">
+        <v>10194.671775360999</v>
+      </c>
+      <c r="H46">
+        <f t="shared" si="0"/>
+        <v>10444.671775360999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>2</v>
       </c>
@@ -7705,8 +8689,15 @@
       <c r="F47">
         <v>10449.470537830101</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G47">
+        <v>10195.026861612399</v>
+      </c>
+      <c r="H47">
+        <f t="shared" si="0"/>
+        <v>10445.026861612399</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>2</v>
       </c>
@@ -7725,8 +8716,15 @@
       <c r="F48">
         <v>10449.297115956701</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G48">
+        <v>10195.2861676581</v>
+      </c>
+      <c r="H48">
+        <f t="shared" si="0"/>
+        <v>10445.2861676581</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>2</v>
       </c>
@@ -7745,8 +8743,15 @@
       <c r="F49">
         <v>10450.614157215599</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G49">
+        <v>10197.898176176401</v>
+      </c>
+      <c r="H49">
+        <f t="shared" si="0"/>
+        <v>10447.898176176401</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>2</v>
       </c>
@@ -7765,8 +8770,15 @@
       <c r="F50">
         <v>10450.4150554588</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G50">
+        <v>10199.3004224214</v>
+      </c>
+      <c r="H50">
+        <f t="shared" si="0"/>
+        <v>10449.3004224214</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>2</v>
       </c>
@@ -7785,8 +8797,15 @@
       <c r="F51">
         <v>10451.442167327999</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G51">
+        <v>10203.6478648471</v>
+      </c>
+      <c r="H51">
+        <f t="shared" si="0"/>
+        <v>10453.6478648471</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>2</v>
       </c>
@@ -7805,8 +8824,15 @@
       <c r="F52">
         <v>10450.8400844159</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G52">
+        <v>10204.9537918487</v>
+      </c>
+      <c r="H52">
+        <f t="shared" si="0"/>
+        <v>10454.9537918487</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>2</v>
       </c>
@@ -7825,8 +8851,15 @@
       <c r="F53">
         <v>10455.8002779163</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G53">
+        <v>10206.598585469401</v>
+      </c>
+      <c r="H53">
+        <f t="shared" si="0"/>
+        <v>10456.598585469401</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>2</v>
       </c>
@@ -7845,8 +8878,15 @@
       <c r="F54">
         <v>10455.373769010301</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G54">
+        <v>10212.9475250449</v>
+      </c>
+      <c r="H54">
+        <f t="shared" si="0"/>
+        <v>10462.9475250449</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>2</v>
       </c>
@@ -7865,8 +8905,15 @@
       <c r="F55">
         <v>10456.193084553801</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G55">
+        <v>10216.2090250244</v>
+      </c>
+      <c r="H55">
+        <f t="shared" si="0"/>
+        <v>10466.2090250244</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>2</v>
       </c>
@@ -7885,8 +8932,15 @@
       <c r="F56">
         <v>10478.3074003534</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G56">
+        <v>10218.672107022499</v>
+      </c>
+      <c r="H56">
+        <f t="shared" si="0"/>
+        <v>10468.672107022499</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>2</v>
       </c>
@@ -7905,8 +8959,15 @@
       <c r="F57">
         <v>10479.526946960101</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G57">
+        <v>10221.0473502516</v>
+      </c>
+      <c r="H57">
+        <f t="shared" si="0"/>
+        <v>10471.0473502516</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>2</v>
       </c>
@@ -7925,8 +8986,15 @@
       <c r="F58">
         <v>10478.936784203401</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G58">
+        <v>10222.0736175498</v>
+      </c>
+      <c r="H58">
+        <f t="shared" si="0"/>
+        <v>10472.0736175498</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>2</v>
       </c>
@@ -7945,8 +9013,15 @@
       <c r="F59">
         <v>10480.4031708967</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G59">
+        <v>10223.4167269397</v>
+      </c>
+      <c r="H59">
+        <f t="shared" si="0"/>
+        <v>10473.4167269397</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>2</v>
       </c>
@@ -7965,8 +9040,15 @@
       <c r="F60">
         <v>10480.2709500773</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G60">
+        <v>10224.797663306101</v>
+      </c>
+      <c r="H60">
+        <f t="shared" si="0"/>
+        <v>10474.797663306101</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>2</v>
       </c>
@@ -7985,8 +9067,15 @@
       <c r="F61">
         <v>10479.336449848501</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G61">
+        <v>10227.181025051799</v>
+      </c>
+      <c r="H61">
+        <f t="shared" si="0"/>
+        <v>10477.181025051799</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>2</v>
       </c>
@@ -8005,8 +9094,15 @@
       <c r="F62">
         <v>10479.106048506001</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G62">
+        <v>10229.0820640689</v>
+      </c>
+      <c r="H62">
+        <f t="shared" si="0"/>
+        <v>10479.0820640689</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>2</v>
       </c>
@@ -8025,8 +9121,15 @@
       <c r="F63">
         <v>10479.752224591401</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G63">
+        <v>10231.137285988299</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="0"/>
+        <v>10481.137285988299</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>2</v>
       </c>
@@ -8045,8 +9148,15 @@
       <c r="F64">
         <v>10479.109017958701</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G64">
+        <v>10231.490956043501</v>
+      </c>
+      <c r="H64">
+        <f t="shared" si="0"/>
+        <v>10481.490956043501</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>2</v>
       </c>
@@ -8065,8 +9175,15 @@
       <c r="F65">
         <v>10480.784807419001</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G65">
+        <v>10234.624123620501</v>
+      </c>
+      <c r="H65">
+        <f t="shared" si="0"/>
+        <v>10484.624123620501</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>2</v>
       </c>
@@ -8085,8 +9202,15 @@
       <c r="F66">
         <v>10480.61603066</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G66">
+        <v>10235.6192069972</v>
+      </c>
+      <c r="H66">
+        <f t="shared" si="0"/>
+        <v>10485.6192069972</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>2</v>
       </c>
@@ -8105,8 +9229,15 @@
       <c r="F67">
         <v>10477.570058158801</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G67">
+        <v>10238.9043390607</v>
+      </c>
+      <c r="H67">
+        <f t="shared" ref="H67:H130" si="1">G67+250</f>
+        <v>10488.9043390607</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>2</v>
       </c>
@@ -8125,8 +9256,15 @@
       <c r="F68">
         <v>10473.2081040618</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G68">
+        <v>10239.8697324719</v>
+      </c>
+      <c r="H68">
+        <f t="shared" si="1"/>
+        <v>10489.8697324719</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>2</v>
       </c>
@@ -8145,8 +9283,15 @@
       <c r="F69">
         <v>10471.684534227899</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G69">
+        <v>10241.4919261345</v>
+      </c>
+      <c r="H69">
+        <f t="shared" si="1"/>
+        <v>10491.4919261345</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>2</v>
       </c>
@@ -8165,8 +9310,15 @@
       <c r="F70">
         <v>10472.398157755901</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G70">
+        <v>10243.3103938843</v>
+      </c>
+      <c r="H70">
+        <f t="shared" si="1"/>
+        <v>10493.3103938843</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>2</v>
       </c>
@@ -8185,8 +9337,15 @@
       <c r="F71">
         <v>10474.191643230701</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G71">
+        <v>10244.3115554263</v>
+      </c>
+      <c r="H71">
+        <f t="shared" si="1"/>
+        <v>10494.3115554263</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>2</v>
       </c>
@@ -8205,8 +9364,15 @@
       <c r="F72">
         <v>10473.5073736992</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G72">
+        <v>10245.6809079923</v>
+      </c>
+      <c r="H72">
+        <f t="shared" si="1"/>
+        <v>10495.6809079923</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>2</v>
       </c>
@@ -8225,8 +9391,15 @@
       <c r="F73">
         <v>10474.999537384099</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G73">
+        <v>10247.722524750599</v>
+      </c>
+      <c r="H73">
+        <f t="shared" si="1"/>
+        <v>10497.722524750599</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>2</v>
       </c>
@@ -8245,8 +9418,15 @@
       <c r="F74">
         <v>10475.6419671039</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G74">
+        <v>10248.822897428699</v>
+      </c>
+      <c r="H74">
+        <f t="shared" si="1"/>
+        <v>10498.822897428699</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>2</v>
       </c>
@@ -8265,8 +9445,15 @@
       <c r="F75">
         <v>10474.5094339853</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G75">
+        <v>10251.8246469969</v>
+      </c>
+      <c r="H75">
+        <f t="shared" si="1"/>
+        <v>10501.8246469969</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>2</v>
       </c>
@@ -8285,8 +9472,15 @@
       <c r="F76">
         <v>10474.436348556899</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G76">
+        <v>10252.110829823099</v>
+      </c>
+      <c r="H76">
+        <f t="shared" si="1"/>
+        <v>10502.110829823099</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>2</v>
       </c>
@@ -8305,8 +9499,15 @@
       <c r="F77">
         <v>10474.792669865499</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G77">
+        <v>10254.996519313399</v>
+      </c>
+      <c r="H77">
+        <f t="shared" si="1"/>
+        <v>10504.996519313399</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>2</v>
       </c>
@@ -8325,8 +9526,15 @@
       <c r="F78">
         <v>10474.7998812282</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G78">
+        <v>10256.841079858999</v>
+      </c>
+      <c r="H78">
+        <f t="shared" si="1"/>
+        <v>10506.841079858999</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>2</v>
       </c>
@@ -8345,8 +9553,15 @@
       <c r="F79">
         <v>10475.0940900448</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G79">
+        <v>10258.4664597889</v>
+      </c>
+      <c r="H79">
+        <f t="shared" si="1"/>
+        <v>10508.4664597889</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>2</v>
       </c>
@@ -8365,8 +9580,15 @@
       <c r="F80">
         <v>10475.764163744399</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G80">
+        <v>10260.5622390523</v>
+      </c>
+      <c r="H80">
+        <f t="shared" si="1"/>
+        <v>10510.5622390523</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>2</v>
       </c>
@@ -8385,8 +9607,15 @@
       <c r="F81">
         <v>10481.961800351501</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G81">
+        <v>10262.4979073418</v>
+      </c>
+      <c r="H81">
+        <f t="shared" si="1"/>
+        <v>10512.4979073418</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>2</v>
       </c>
@@ -8405,8 +9634,15 @@
       <c r="F82">
         <v>10482.410744565501</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G82">
+        <v>10263.255799903</v>
+      </c>
+      <c r="H82">
+        <f t="shared" si="1"/>
+        <v>10513.255799903</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>2</v>
       </c>
@@ -8425,8 +9661,15 @@
       <c r="F83">
         <v>10482.624430154199</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G83">
+        <v>10263.5369620276</v>
+      </c>
+      <c r="H83">
+        <f t="shared" si="1"/>
+        <v>10513.5369620276</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>2</v>
       </c>
@@ -8445,8 +9688,15 @@
       <c r="F84">
         <v>10484.047358947901</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G84">
+        <v>10264.8513878386</v>
+      </c>
+      <c r="H84">
+        <f t="shared" si="1"/>
+        <v>10514.8513878386</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>2</v>
       </c>
@@ -8465,8 +9715,15 @@
       <c r="F85">
         <v>10520.905369367299</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G85">
+        <v>10267.5707432992</v>
+      </c>
+      <c r="H85">
+        <f t="shared" si="1"/>
+        <v>10517.5707432992</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>2</v>
       </c>
@@ -8485,8 +9742,15 @@
       <c r="F86">
         <v>10521.806549084</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G86">
+        <v>10269.7681720949</v>
+      </c>
+      <c r="H86">
+        <f t="shared" si="1"/>
+        <v>10519.7681720949</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>2</v>
       </c>
@@ -8505,8 +9769,15 @@
       <c r="F87">
         <v>10522.3431883137</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G87">
+        <v>10271.828701767499</v>
+      </c>
+      <c r="H87">
+        <f t="shared" si="1"/>
+        <v>10521.828701767499</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>2</v>
       </c>
@@ -8525,8 +9796,15 @@
       <c r="F88">
         <v>10520.623859096801</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G88">
+        <v>10272.840250564799</v>
+      </c>
+      <c r="H88">
+        <f t="shared" si="1"/>
+        <v>10522.840250564799</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>2</v>
       </c>
@@ -8545,8 +9823,15 @@
       <c r="F89">
         <v>10524.886639639</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G89">
+        <v>10275.5392716729</v>
+      </c>
+      <c r="H89">
+        <f t="shared" si="1"/>
+        <v>10525.5392716729</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>2</v>
       </c>
@@ -8565,8 +9850,15 @@
       <c r="F90">
         <v>10525.8713123497</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G90">
+        <v>10277.6970693888</v>
+      </c>
+      <c r="H90">
+        <f t="shared" si="1"/>
+        <v>10527.6970693888</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>2</v>
       </c>
@@ -8585,8 +9877,15 @@
       <c r="F91">
         <v>10525.5030961264</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G91">
+        <v>10280.3730581666</v>
+      </c>
+      <c r="H91">
+        <f t="shared" si="1"/>
+        <v>10530.3730581666</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>2</v>
       </c>
@@ -8605,8 +9904,15 @@
       <c r="F92">
         <v>10550.6803149023</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G92">
+        <v>10282.220688085699</v>
+      </c>
+      <c r="H92">
+        <f t="shared" si="1"/>
+        <v>10532.220688085699</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>2</v>
       </c>
@@ -8625,8 +9931,15 @@
       <c r="F93">
         <v>10554.1388776318</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G93">
+        <v>10287.382520401999</v>
+      </c>
+      <c r="H93">
+        <f t="shared" si="1"/>
+        <v>10537.382520401999</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>2</v>
       </c>
@@ -8645,8 +9958,15 @@
       <c r="F94">
         <v>10554.0380615797</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G94">
+        <v>10287.0201261163</v>
+      </c>
+      <c r="H94">
+        <f t="shared" si="1"/>
+        <v>10537.0201261163</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>2</v>
       </c>
@@ -8665,8 +9985,15 @@
       <c r="F95">
         <v>10554.955047715001</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G95">
+        <v>10289.343660242899</v>
+      </c>
+      <c r="H95">
+        <f t="shared" si="1"/>
+        <v>10539.343660242899</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>2</v>
       </c>
@@ -8685,8 +10012,15 @@
       <c r="F96">
         <v>10555.2559467273</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G96">
+        <v>10291.0924515684</v>
+      </c>
+      <c r="H96">
+        <f t="shared" si="1"/>
+        <v>10541.0924515684</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>2</v>
       </c>
@@ -8705,8 +10039,15 @@
       <c r="F97">
         <v>10554.895226147501</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G97">
+        <v>10294.077044742</v>
+      </c>
+      <c r="H97">
+        <f t="shared" si="1"/>
+        <v>10544.077044742</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>2</v>
       </c>
@@ -8725,8 +10066,15 @@
       <c r="F98">
         <v>10555.506256483601</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G98">
+        <v>10294.9792953412</v>
+      </c>
+      <c r="H98">
+        <f t="shared" si="1"/>
+        <v>10544.9792953412</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>2</v>
       </c>
@@ -8745,8 +10093,15 @@
       <c r="F99">
         <v>10554.015022662899</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G99">
+        <v>10295.0147771591</v>
+      </c>
+      <c r="H99">
+        <f t="shared" si="1"/>
+        <v>10545.0147771591</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>2</v>
       </c>
@@ -8765,8 +10120,15 @@
       <c r="F100">
         <v>10554.6993727237</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G100">
+        <v>10297.528430341899</v>
+      </c>
+      <c r="H100">
+        <f t="shared" si="1"/>
+        <v>10547.528430341899</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>2</v>
       </c>
@@ -8785,8 +10147,15 @@
       <c r="F101">
         <v>10555.606978240799</v>
       </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G101">
+        <v>10304.752923951401</v>
+      </c>
+      <c r="H101">
+        <f t="shared" si="1"/>
+        <v>10554.752923951401</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>2</v>
       </c>
@@ -8805,8 +10174,15 @@
       <c r="F102">
         <v>10557.214445228299</v>
       </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G102">
+        <v>10305.969206984701</v>
+      </c>
+      <c r="H102">
+        <f t="shared" si="1"/>
+        <v>10555.969206984701</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>2</v>
       </c>
@@ -8825,8 +10201,15 @@
       <c r="F103">
         <v>10556.796785456399</v>
       </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G103">
+        <v>10306.539899203401</v>
+      </c>
+      <c r="H103">
+        <f t="shared" si="1"/>
+        <v>10556.539899203401</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>2</v>
       </c>
@@ -8845,8 +10228,15 @@
       <c r="F104">
         <v>10556.239461338801</v>
       </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G104">
+        <v>10310.171561777501</v>
+      </c>
+      <c r="H104">
+        <f t="shared" si="1"/>
+        <v>10560.171561777501</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>2</v>
       </c>
@@ -8865,8 +10255,15 @@
       <c r="F105">
         <v>10556.156450201501</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G105">
+        <v>10310.027477101299</v>
+      </c>
+      <c r="H105">
+        <f t="shared" si="1"/>
+        <v>10560.027477101299</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>2</v>
       </c>
@@ -8885,8 +10282,15 @@
       <c r="F106">
         <v>10555.4075258788</v>
       </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G106">
+        <v>10312.5038857241</v>
+      </c>
+      <c r="H106">
+        <f t="shared" si="1"/>
+        <v>10562.5038857241</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>2</v>
       </c>
@@ -8905,8 +10309,15 @@
       <c r="F107">
         <v>10558.6444544156</v>
       </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G107">
+        <v>10314.344527584601</v>
+      </c>
+      <c r="H107">
+        <f t="shared" si="1"/>
+        <v>10564.344527584601</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>2</v>
       </c>
@@ -8925,8 +10336,15 @@
       <c r="F108">
         <v>10557.707048013501</v>
       </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G108">
+        <v>10316.096586939801</v>
+      </c>
+      <c r="H108">
+        <f t="shared" si="1"/>
+        <v>10566.096586939801</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>2</v>
       </c>
@@ -8945,8 +10363,15 @@
       <c r="F109">
         <v>10556.5465436268</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G109">
+        <v>10316.675593088699</v>
+      </c>
+      <c r="H109">
+        <f t="shared" si="1"/>
+        <v>10566.675593088699</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>2</v>
       </c>
@@ -8965,8 +10390,15 @@
       <c r="F110">
         <v>10556.1758770242</v>
       </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G110">
+        <v>10318.1965946981</v>
+      </c>
+      <c r="H110">
+        <f t="shared" si="1"/>
+        <v>10568.1965946981</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>2</v>
       </c>
@@ -8985,8 +10417,15 @@
       <c r="F111">
         <v>10561.973799834501</v>
       </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G111">
+        <v>10318.949248574199</v>
+      </c>
+      <c r="H111">
+        <f t="shared" si="1"/>
+        <v>10568.949248574199</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>2</v>
       </c>
@@ -9005,8 +10444,15 @@
       <c r="F112">
         <v>10562.116124175</v>
       </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G112">
+        <v>10322.575064028801</v>
+      </c>
+      <c r="H112">
+        <f t="shared" si="1"/>
+        <v>10572.575064028801</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>2</v>
       </c>
@@ -9025,8 +10471,15 @@
       <c r="F113">
         <v>10561.978666754299</v>
       </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G113">
+        <v>10323.9884536676</v>
+      </c>
+      <c r="H113">
+        <f t="shared" si="1"/>
+        <v>10573.9884536676</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>2</v>
       </c>
@@ -9045,8 +10498,15 @@
       <c r="F114">
         <v>10565.044106768801</v>
       </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G114">
+        <v>10325.1337880561</v>
+      </c>
+      <c r="H114">
+        <f t="shared" si="1"/>
+        <v>10575.1337880561</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>2</v>
       </c>
@@ -9065,8 +10525,15 @@
       <c r="F115">
         <v>10564.761608514</v>
       </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G115">
+        <v>10325.5685118662</v>
+      </c>
+      <c r="H115">
+        <f t="shared" si="1"/>
+        <v>10575.5685118662</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>2</v>
       </c>
@@ -9085,8 +10552,15 @@
       <c r="F116">
         <v>10564.8918313754</v>
       </c>
-    </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G116">
+        <v>10328.3999890135</v>
+      </c>
+      <c r="H116">
+        <f t="shared" si="1"/>
+        <v>10578.3999890135</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>2</v>
       </c>
@@ -9105,8 +10579,15 @@
       <c r="F117">
         <v>10564.3101936236</v>
       </c>
-    </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G117">
+        <v>10334.2928116802</v>
+      </c>
+      <c r="H117">
+        <f t="shared" si="1"/>
+        <v>10584.2928116802</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>2</v>
       </c>
@@ -9125,8 +10606,15 @@
       <c r="F118">
         <v>10564.2295238674</v>
       </c>
-    </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G118">
+        <v>10337.298214152999</v>
+      </c>
+      <c r="H118">
+        <f t="shared" si="1"/>
+        <v>10587.298214152999</v>
+      </c>
+    </row>
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>2</v>
       </c>
@@ -9145,8 +10633,15 @@
       <c r="F119">
         <v>10596.2084825813</v>
       </c>
-    </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G119">
+        <v>10338.9876178268</v>
+      </c>
+      <c r="H119">
+        <f t="shared" si="1"/>
+        <v>10588.9876178268</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>2</v>
       </c>
@@ -9165,8 +10660,15 @@
       <c r="F120">
         <v>10627.5167173228</v>
       </c>
-    </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G120">
+        <v>10342.542461840399</v>
+      </c>
+      <c r="H120">
+        <f t="shared" si="1"/>
+        <v>10592.542461840399</v>
+      </c>
+    </row>
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>2</v>
       </c>
@@ -9185,8 +10687,15 @@
       <c r="F121">
         <v>10629.877980711801</v>
       </c>
-    </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G121">
+        <v>10344.9635867711</v>
+      </c>
+      <c r="H121">
+        <f t="shared" si="1"/>
+        <v>10594.9635867711</v>
+      </c>
+    </row>
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>2</v>
       </c>
@@ -9205,8 +10714,15 @@
       <c r="F122">
         <v>10630.4037998615</v>
       </c>
-    </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G122">
+        <v>10348.767489850699</v>
+      </c>
+      <c r="H122">
+        <f t="shared" si="1"/>
+        <v>10598.767489850699</v>
+      </c>
+    </row>
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>2</v>
       </c>
@@ -9225,8 +10741,15 @@
       <c r="F123">
         <v>10621.917678273399</v>
       </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G123">
+        <v>10350.1570545782</v>
+      </c>
+      <c r="H123">
+        <f t="shared" si="1"/>
+        <v>10600.1570545782</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>2</v>
       </c>
@@ -9245,8 +10768,15 @@
       <c r="F124">
         <v>10623.5700053289</v>
       </c>
-    </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G124">
+        <v>10353.480684903099</v>
+      </c>
+      <c r="H124">
+        <f t="shared" si="1"/>
+        <v>10603.480684903099</v>
+      </c>
+    </row>
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>2</v>
       </c>
@@ -9265,8 +10795,15 @@
       <c r="F125">
         <v>10623.719714602399</v>
       </c>
-    </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G125">
+        <v>10355.8003239725</v>
+      </c>
+      <c r="H125">
+        <f t="shared" si="1"/>
+        <v>10605.8003239725</v>
+      </c>
+    </row>
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>2</v>
       </c>
@@ -9285,8 +10822,15 @@
       <c r="F126">
         <v>10624.4387443491</v>
       </c>
-    </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G126">
+        <v>10359.603456565201</v>
+      </c>
+      <c r="H126">
+        <f t="shared" si="1"/>
+        <v>10609.603456565201</v>
+      </c>
+    </row>
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>2</v>
       </c>
@@ -9305,8 +10849,15 @@
       <c r="F127">
         <v>10623.755755713701</v>
       </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G127">
+        <v>10359.999239895</v>
+      </c>
+      <c r="H127">
+        <f t="shared" si="1"/>
+        <v>10609.999239895</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>2</v>
       </c>
@@ -9325,8 +10876,15 @@
       <c r="F128">
         <v>10623.2176227411</v>
       </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G128">
+        <v>10362.603643853099</v>
+      </c>
+      <c r="H128">
+        <f t="shared" si="1"/>
+        <v>10612.603643853099</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>2</v>
       </c>
@@ -9345,8 +10903,15 @@
       <c r="F129">
         <v>10633.409253154499</v>
       </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G129">
+        <v>10364.9456265115</v>
+      </c>
+      <c r="H129">
+        <f t="shared" si="1"/>
+        <v>10614.9456265115</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>2</v>
       </c>
@@ -9365,8 +10930,15 @@
       <c r="F130">
         <v>10632.4278789372</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G130">
+        <v>10367.4443818871</v>
+      </c>
+      <c r="H130">
+        <f t="shared" si="1"/>
+        <v>10617.4443818871</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>2</v>
       </c>
@@ -9385,8 +10957,15 @@
       <c r="F131">
         <v>10636.477800524601</v>
       </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G131">
+        <v>10368.9008909686</v>
+      </c>
+      <c r="H131">
+        <f t="shared" ref="H131:H194" si="2">G131+250</f>
+        <v>10618.9008909686</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>2</v>
       </c>
@@ -9405,8 +10984,15 @@
       <c r="F132">
         <v>10637.8544688048</v>
       </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G132">
+        <v>10370.978256724</v>
+      </c>
+      <c r="H132">
+        <f t="shared" si="2"/>
+        <v>10620.978256724</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>2</v>
       </c>
@@ -9425,8 +11011,15 @@
       <c r="F133">
         <v>10636.5915098309</v>
       </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G133">
+        <v>10370.606307488601</v>
+      </c>
+      <c r="H133">
+        <f t="shared" si="2"/>
+        <v>10620.606307488601</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>2</v>
       </c>
@@ -9445,8 +11038,15 @@
       <c r="F134">
         <v>10637.503333004401</v>
       </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G134">
+        <v>10373.681531623</v>
+      </c>
+      <c r="H134">
+        <f t="shared" si="2"/>
+        <v>10623.681531623</v>
+      </c>
+    </row>
+    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>2</v>
       </c>
@@ -9465,8 +11065,15 @@
       <c r="F135">
         <v>10637.7331271903</v>
       </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G135">
+        <v>10374.504665611799</v>
+      </c>
+      <c r="H135">
+        <f t="shared" si="2"/>
+        <v>10624.504665611799</v>
+      </c>
+    </row>
+    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>2</v>
       </c>
@@ -9485,8 +11092,15 @@
       <c r="F136">
         <v>10640.313399381699</v>
       </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G136">
+        <v>10376.782421722201</v>
+      </c>
+      <c r="H136">
+        <f t="shared" si="2"/>
+        <v>10626.782421722201</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>2</v>
       </c>
@@ -9505,8 +11119,15 @@
       <c r="F137">
         <v>10640.991478657699</v>
       </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G137">
+        <v>10377.856266660399</v>
+      </c>
+      <c r="H137">
+        <f t="shared" si="2"/>
+        <v>10627.856266660399</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>2</v>
       </c>
@@ -9525,8 +11146,15 @@
       <c r="F138">
         <v>10642.3718635287</v>
       </c>
-    </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G138">
+        <v>10380.716666599499</v>
+      </c>
+      <c r="H138">
+        <f t="shared" si="2"/>
+        <v>10630.716666599499</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>2</v>
       </c>
@@ -9545,8 +11173,15 @@
       <c r="F139">
         <v>10645.3342502138</v>
       </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G139">
+        <v>10382.4224503655</v>
+      </c>
+      <c r="H139">
+        <f t="shared" si="2"/>
+        <v>10632.4224503655</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>2</v>
       </c>
@@ -9565,8 +11200,15 @@
       <c r="F140">
         <v>10645.1638161673</v>
       </c>
-    </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G140">
+        <v>10382.8886949358</v>
+      </c>
+      <c r="H140">
+        <f t="shared" si="2"/>
+        <v>10632.8886949358</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>2</v>
       </c>
@@ -9585,8 +11227,15 @@
       <c r="F141">
         <v>10644.525646558899</v>
       </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G141">
+        <v>10382.758545761901</v>
+      </c>
+      <c r="H141">
+        <f t="shared" si="2"/>
+        <v>10632.758545761901</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>2</v>
       </c>
@@ -9605,8 +11254,15 @@
       <c r="F142">
         <v>10644.259332682999</v>
       </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G142">
+        <v>10384.4230431625</v>
+      </c>
+      <c r="H142">
+        <f t="shared" si="2"/>
+        <v>10634.4230431625</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>2</v>
       </c>
@@ -9625,8 +11281,15 @@
       <c r="F143">
         <v>10644.0828586141</v>
       </c>
-    </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G143">
+        <v>10387.8157569714</v>
+      </c>
+      <c r="H143">
+        <f t="shared" si="2"/>
+        <v>10637.8157569714</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>2</v>
       </c>
@@ -9645,8 +11308,15 @@
       <c r="F144">
         <v>10644.168403656</v>
       </c>
-    </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G144">
+        <v>10389.971251504399</v>
+      </c>
+      <c r="H144">
+        <f t="shared" si="2"/>
+        <v>10639.971251504399</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>2</v>
       </c>
@@ -9665,8 +11335,15 @@
       <c r="F145">
         <v>10644.414789361699</v>
       </c>
-    </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G145">
+        <v>10393.3374825174</v>
+      </c>
+      <c r="H145">
+        <f t="shared" si="2"/>
+        <v>10643.3374825174</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>2</v>
       </c>
@@ -9685,8 +11362,15 @@
       <c r="F146">
         <v>10644.317601373899</v>
       </c>
-    </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G146">
+        <v>10397.2473597341</v>
+      </c>
+      <c r="H146">
+        <f t="shared" si="2"/>
+        <v>10647.2473597341</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>2</v>
       </c>
@@ -9705,8 +11389,15 @@
       <c r="F147">
         <v>10644.530325747901</v>
       </c>
-    </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G147">
+        <v>10398.3713028494</v>
+      </c>
+      <c r="H147">
+        <f t="shared" si="2"/>
+        <v>10648.3713028494</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>2</v>
       </c>
@@ -9725,8 +11416,15 @@
       <c r="F148">
         <v>10645.779636760501</v>
       </c>
-    </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G148">
+        <v>10402.5779359758</v>
+      </c>
+      <c r="H148">
+        <f t="shared" si="2"/>
+        <v>10652.5779359758</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>2</v>
       </c>
@@ -9745,8 +11443,15 @@
       <c r="F149">
         <v>10645.085018911799</v>
       </c>
-    </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G149">
+        <v>10401.638711788701</v>
+      </c>
+      <c r="H149">
+        <f t="shared" si="2"/>
+        <v>10651.638711788701</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>2</v>
       </c>
@@ -9765,8 +11470,15 @@
       <c r="F150">
         <v>10642.107604123201</v>
       </c>
-    </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G150">
+        <v>10402.617326940401</v>
+      </c>
+      <c r="H150">
+        <f t="shared" si="2"/>
+        <v>10652.617326940401</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>2</v>
       </c>
@@ -9785,8 +11497,15 @@
       <c r="F151">
         <v>10642.5236590843</v>
       </c>
-    </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G151">
+        <v>10403.339929924799</v>
+      </c>
+      <c r="H151">
+        <f t="shared" si="2"/>
+        <v>10653.339929924799</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>2</v>
       </c>
@@ -9805,8 +11524,15 @@
       <c r="F152">
         <v>10643.6640895741</v>
       </c>
-    </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G152">
+        <v>10405.5663599255</v>
+      </c>
+      <c r="H152">
+        <f t="shared" si="2"/>
+        <v>10655.5663599255</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>2</v>
       </c>
@@ -9825,8 +11551,15 @@
       <c r="F153">
         <v>10643.2192136999</v>
       </c>
-    </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G153">
+        <v>10407.1692824561</v>
+      </c>
+      <c r="H153">
+        <f t="shared" si="2"/>
+        <v>10657.1692824561</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>2</v>
       </c>
@@ -9845,8 +11578,15 @@
       <c r="F154">
         <v>10644.504842037801</v>
       </c>
-    </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G154">
+        <v>10409.2619717746</v>
+      </c>
+      <c r="H154">
+        <f t="shared" si="2"/>
+        <v>10659.2619717746</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>2</v>
       </c>
@@ -9865,8 +11605,15 @@
       <c r="F155">
         <v>10648.9160693752</v>
       </c>
-    </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G155">
+        <v>10412.523529529301</v>
+      </c>
+      <c r="H155">
+        <f t="shared" si="2"/>
+        <v>10662.523529529301</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>2</v>
       </c>
@@ -9885,8 +11632,15 @@
       <c r="F156">
         <v>10647.3111561316</v>
       </c>
-    </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G156">
+        <v>10412.0962361152</v>
+      </c>
+      <c r="H156">
+        <f t="shared" si="2"/>
+        <v>10662.0962361152</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>2</v>
       </c>
@@ -9905,8 +11659,15 @@
       <c r="F157">
         <v>10700.7963301034</v>
       </c>
-    </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G157">
+        <v>10414.2135989013</v>
+      </c>
+      <c r="H157">
+        <f t="shared" si="2"/>
+        <v>10664.2135989013</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>2</v>
       </c>
@@ -9925,8 +11686,15 @@
       <c r="F158">
         <v>10701.51334143</v>
       </c>
-    </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G158">
+        <v>10415.2456187099</v>
+      </c>
+      <c r="H158">
+        <f t="shared" si="2"/>
+        <v>10665.2456187099</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>2</v>
       </c>
@@ -9945,8 +11713,15 @@
       <c r="F159">
         <v>10708.2702288981</v>
       </c>
-    </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G159">
+        <v>10417.683503717501</v>
+      </c>
+      <c r="H159">
+        <f t="shared" si="2"/>
+        <v>10667.683503717501</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>2</v>
       </c>
@@ -9965,8 +11740,15 @@
       <c r="F160">
         <v>10707.426942497101</v>
       </c>
-    </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G160">
+        <v>10417.6849614695</v>
+      </c>
+      <c r="H160">
+        <f t="shared" si="2"/>
+        <v>10667.6849614695</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>2</v>
       </c>
@@ -9985,8 +11767,15 @@
       <c r="F161">
         <v>10706.7105930131</v>
       </c>
-    </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G161">
+        <v>10419.072136762599</v>
+      </c>
+      <c r="H161">
+        <f t="shared" si="2"/>
+        <v>10669.072136762599</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>2</v>
       </c>
@@ -10005,8 +11794,15 @@
       <c r="F162">
         <v>10706.7283525987</v>
       </c>
-    </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G162">
+        <v>10420.910868978401</v>
+      </c>
+      <c r="H162">
+        <f t="shared" si="2"/>
+        <v>10670.910868978401</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>2</v>
       </c>
@@ -10025,8 +11821,15 @@
       <c r="F163">
         <v>10706.975606579599</v>
       </c>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G163">
+        <v>10423.4412289885</v>
+      </c>
+      <c r="H163">
+        <f t="shared" si="2"/>
+        <v>10673.4412289885</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164">
         <v>2</v>
       </c>
@@ -10045,8 +11848,15 @@
       <c r="F164">
         <v>10707.724428531699</v>
       </c>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G164">
+        <v>10424.3086405269</v>
+      </c>
+      <c r="H164">
+        <f t="shared" si="2"/>
+        <v>10674.3086405269</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A165">
         <v>2</v>
       </c>
@@ -10065,8 +11875,15 @@
       <c r="F165">
         <v>10708.955089651099</v>
       </c>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G165">
+        <v>10425.7055090699</v>
+      </c>
+      <c r="H165">
+        <f t="shared" si="2"/>
+        <v>10675.7055090699</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A166">
         <v>2</v>
       </c>
@@ -10085,8 +11902,15 @@
       <c r="F166">
         <v>10708.731679824599</v>
       </c>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G166">
+        <v>10429.6833434032</v>
+      </c>
+      <c r="H166">
+        <f t="shared" si="2"/>
+        <v>10679.6833434032</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A167">
         <v>2</v>
       </c>
@@ -10105,8 +11929,15 @@
       <c r="F167">
         <v>10708.2840575143</v>
       </c>
-    </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G167">
+        <v>10430.994719037701</v>
+      </c>
+      <c r="H167">
+        <f t="shared" si="2"/>
+        <v>10680.994719037701</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A168">
         <v>2</v>
       </c>
@@ -10125,8 +11956,15 @@
       <c r="F168">
         <v>10707.7984945035</v>
       </c>
-    </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G168">
+        <v>10431.571631062199</v>
+      </c>
+      <c r="H168">
+        <f t="shared" si="2"/>
+        <v>10681.571631062199</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A169">
         <v>2</v>
       </c>
@@ -10145,8 +11983,15 @@
       <c r="F169">
         <v>10716.1606525609</v>
       </c>
-    </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G169">
+        <v>10433.7683958903</v>
+      </c>
+      <c r="H169">
+        <f t="shared" si="2"/>
+        <v>10683.7683958903</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A170">
         <v>2</v>
       </c>
@@ -10165,8 +12010,15 @@
       <c r="F170">
         <v>10716.775486647801</v>
       </c>
-    </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G170">
+        <v>10436.455650457799</v>
+      </c>
+      <c r="H170">
+        <f t="shared" si="2"/>
+        <v>10686.455650457799</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A171">
         <v>2</v>
       </c>
@@ -10185,8 +12037,15 @@
       <c r="F171">
         <v>10715.7876610204</v>
       </c>
-    </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G171">
+        <v>10437.7873299864</v>
+      </c>
+      <c r="H171">
+        <f t="shared" si="2"/>
+        <v>10687.7873299864</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A172">
         <v>2</v>
       </c>
@@ -10205,8 +12064,15 @@
       <c r="F172">
         <v>10716.2584983581</v>
       </c>
-    </row>
-    <row r="173" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G172">
+        <v>10439.100630765401</v>
+      </c>
+      <c r="H172">
+        <f t="shared" si="2"/>
+        <v>10689.100630765401</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173">
         <v>2</v>
       </c>
@@ -10225,8 +12091,15 @@
       <c r="F173">
         <v>10716.7888659254</v>
       </c>
-    </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G173">
+        <v>10438.6638213608</v>
+      </c>
+      <c r="H173">
+        <f t="shared" si="2"/>
+        <v>10688.6638213608</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174">
         <v>2</v>
       </c>
@@ -10245,8 +12118,15 @@
       <c r="F174">
         <v>10717.160703220699</v>
       </c>
-    </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G174">
+        <v>10441.6303143202</v>
+      </c>
+      <c r="H174">
+        <f t="shared" si="2"/>
+        <v>10691.6303143202</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175">
         <v>2</v>
       </c>
@@ -10265,8 +12145,15 @@
       <c r="F175">
         <v>10722.6655208347</v>
       </c>
-    </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G175">
+        <v>10443.5487349295</v>
+      </c>
+      <c r="H175">
+        <f t="shared" si="2"/>
+        <v>10693.5487349295</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A176">
         <v>2</v>
       </c>
@@ -10285,8 +12172,15 @@
       <c r="F176">
         <v>10722.484930438801</v>
       </c>
-    </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G176">
+        <v>10444.6362803506</v>
+      </c>
+      <c r="H176">
+        <f t="shared" si="2"/>
+        <v>10694.6362803506</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A177">
         <v>2</v>
       </c>
@@ -10305,8 +12199,15 @@
       <c r="F177">
         <v>10722.285252199201</v>
       </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G177">
+        <v>10444.104440569699</v>
+      </c>
+      <c r="H177">
+        <f t="shared" si="2"/>
+        <v>10694.104440569699</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178">
         <v>2</v>
       </c>
@@ -10325,8 +12226,15 @@
       <c r="F178">
         <v>10722.826321479601</v>
       </c>
-    </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G178">
+        <v>10446.295503564699</v>
+      </c>
+      <c r="H178">
+        <f t="shared" si="2"/>
+        <v>10696.295503564699</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179">
         <v>2</v>
       </c>
@@ -10345,8 +12253,15 @@
       <c r="F179">
         <v>10722.8173042046</v>
       </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G179">
+        <v>10447.824409697099</v>
+      </c>
+      <c r="H179">
+        <f t="shared" si="2"/>
+        <v>10697.824409697099</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A180">
         <v>2</v>
       </c>
@@ -10365,8 +12280,15 @@
       <c r="F180">
         <v>10722.4802927119</v>
       </c>
-    </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G180">
+        <v>10448.645411998101</v>
+      </c>
+      <c r="H180">
+        <f t="shared" si="2"/>
+        <v>10698.645411998101</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181">
         <v>2</v>
       </c>
@@ -10385,8 +12307,15 @@
       <c r="F181">
         <v>10721.7772686565</v>
       </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G181">
+        <v>10448.680845298</v>
+      </c>
+      <c r="H181">
+        <f t="shared" si="2"/>
+        <v>10698.680845298</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182">
         <v>2</v>
       </c>
@@ -10405,8 +12334,15 @@
       <c r="F182">
         <v>10717.0452679027</v>
       </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G182">
+        <v>10450.373830722099</v>
+      </c>
+      <c r="H182">
+        <f t="shared" si="2"/>
+        <v>10700.373830722099</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A183">
         <v>2</v>
       </c>
@@ -10425,8 +12361,15 @@
       <c r="F183">
         <v>10718.146853804999</v>
       </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G183">
+        <v>10452.8365372587</v>
+      </c>
+      <c r="H183">
+        <f t="shared" si="2"/>
+        <v>10702.8365372587</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A184">
         <v>2</v>
       </c>
@@ -10445,8 +12388,15 @@
       <c r="F184">
         <v>10717.9041679415</v>
       </c>
-    </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G184">
+        <v>10469.207615003899</v>
+      </c>
+      <c r="H184">
+        <f t="shared" si="2"/>
+        <v>10719.207615003899</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A185">
         <v>2</v>
       </c>
@@ -10465,8 +12415,15 @@
       <c r="F185">
         <v>10718.6818782101</v>
       </c>
-    </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G185">
+        <v>10470.083836741</v>
+      </c>
+      <c r="H185">
+        <f t="shared" si="2"/>
+        <v>10720.083836741</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A186">
         <v>2</v>
       </c>
@@ -10485,8 +12442,15 @@
       <c r="F186">
         <v>10779.174213140999</v>
       </c>
-    </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G186">
+        <v>10472.3239580684</v>
+      </c>
+      <c r="H186">
+        <f t="shared" si="2"/>
+        <v>10722.3239580684</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187">
         <v>2</v>
       </c>
@@ -10505,8 +12469,15 @@
       <c r="F187">
         <v>10785.4111289306</v>
       </c>
-    </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G187">
+        <v>10475.802054919101</v>
+      </c>
+      <c r="H187">
+        <f t="shared" si="2"/>
+        <v>10725.802054919101</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188">
         <v>2</v>
       </c>
@@ -10525,8 +12496,15 @@
       <c r="F188">
         <v>10792.7061883069</v>
       </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G188">
+        <v>10479.3646399017</v>
+      </c>
+      <c r="H188">
+        <f t="shared" si="2"/>
+        <v>10729.3646399017</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189">
         <v>2</v>
       </c>
@@ -10545,8 +12523,15 @@
       <c r="F189">
         <v>10794.9765047948</v>
       </c>
-    </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G189">
+        <v>10483.0556590214</v>
+      </c>
+      <c r="H189">
+        <f t="shared" si="2"/>
+        <v>10733.0556590214</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190">
         <v>2</v>
       </c>
@@ -10565,8 +12550,15 @@
       <c r="F190">
         <v>10794.9549042864</v>
       </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G190">
+        <v>10485.286108345301</v>
+      </c>
+      <c r="H190">
+        <f t="shared" si="2"/>
+        <v>10735.286108345301</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A191">
         <v>2</v>
       </c>
@@ -10585,8 +12577,15 @@
       <c r="F191">
         <v>10794.2185988935</v>
       </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G191">
+        <v>10486.0186487343</v>
+      </c>
+      <c r="H191">
+        <f t="shared" si="2"/>
+        <v>10736.0186487343</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A192">
         <v>2</v>
       </c>
@@ -10605,8 +12604,15 @@
       <c r="F192">
         <v>10796.822543669299</v>
       </c>
-    </row>
-    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G192">
+        <v>10487.626864178899</v>
+      </c>
+      <c r="H192">
+        <f t="shared" si="2"/>
+        <v>10737.626864178899</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193">
         <v>2</v>
       </c>
@@ -10625,8 +12631,15 @@
       <c r="F193">
         <v>10797.1590816182</v>
       </c>
-    </row>
-    <row r="194" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G193">
+        <v>10490.9001293487</v>
+      </c>
+      <c r="H193">
+        <f t="shared" si="2"/>
+        <v>10740.9001293487</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194">
         <v>2</v>
       </c>
@@ -10645,8 +12658,15 @@
       <c r="F194">
         <v>10796.7013735623</v>
       </c>
-    </row>
-    <row r="195" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G194">
+        <v>10491.4825528355</v>
+      </c>
+      <c r="H194">
+        <f t="shared" si="2"/>
+        <v>10741.4825528355</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A195">
         <v>2</v>
       </c>
@@ -10665,8 +12685,15 @@
       <c r="F195">
         <v>10796.781890718699</v>
       </c>
-    </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G195">
+        <v>10492.285455421699</v>
+      </c>
+      <c r="H195">
+        <f t="shared" ref="H195:H201" si="3">G195+250</f>
+        <v>10742.285455421699</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A196">
         <v>2</v>
       </c>
@@ -10685,8 +12712,15 @@
       <c r="F196">
         <v>10798.8307329039</v>
       </c>
-    </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G196">
+        <v>10498.6540684875</v>
+      </c>
+      <c r="H196">
+        <f t="shared" si="3"/>
+        <v>10748.6540684875</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A197">
         <v>2</v>
       </c>
@@ -10705,8 +12739,15 @@
       <c r="F197">
         <v>10798.811221961099</v>
       </c>
-    </row>
-    <row r="198" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G197">
+        <v>10501.3522980869</v>
+      </c>
+      <c r="H197">
+        <f t="shared" si="3"/>
+        <v>10751.3522980869</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A198">
         <v>2</v>
       </c>
@@ -10725,8 +12766,15 @@
       <c r="F198">
         <v>10798.637372506</v>
       </c>
-    </row>
-    <row r="199" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G198">
+        <v>10502.242887620199</v>
+      </c>
+      <c r="H198">
+        <f t="shared" si="3"/>
+        <v>10752.242887620199</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A199">
         <v>2</v>
       </c>
@@ -10745,8 +12793,15 @@
       <c r="F199">
         <v>10798.635218134399</v>
       </c>
-    </row>
-    <row r="200" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G199">
+        <v>10504.678460952</v>
+      </c>
+      <c r="H199">
+        <f t="shared" si="3"/>
+        <v>10754.678460952</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A200">
         <v>2</v>
       </c>
@@ -10765,8 +12820,15 @@
       <c r="F200">
         <v>10801.377138322399</v>
       </c>
-    </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G200">
+        <v>10506.483021178499</v>
+      </c>
+      <c r="H200">
+        <f t="shared" si="3"/>
+        <v>10756.483021178499</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A201">
         <v>2</v>
       </c>
@@ -10784,6 +12846,13 @@
       </c>
       <c r="F201">
         <v>10802.2665196449</v>
+      </c>
+      <c r="G201">
+        <v>10509.171333975901</v>
+      </c>
+      <c r="H201">
+        <f t="shared" si="3"/>
+        <v>10759.171333975901</v>
       </c>
     </row>
   </sheetData>

</xml_diff>